<commit_message>
Added testing broken links
</commit_message>
<xml_diff>
--- a/TestBench/TestData/UIData2.xlsx
+++ b/TestBench/TestData/UIData2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdoppalapudi\Desktop\KT\Automation\TestNGrepo\TestBench\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CA9FD1-1AC4-4691-BD3A-F53BD887AF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C8F7A8-7329-4372-BDF1-98F4D6C9C118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>